<commit_message>
Broken merge commit from master
</commit_message>
<xml_diff>
--- a/Source/Libraries/Core/Business/Vodovoz.Reports/Reports/Logistic/CarsExploitationReport-ConditionalFormatting.xlsx
+++ b/Source/Libraries/Core/Business/Vodovoz.Reports/Reports/Logistic/CarsExploitationReport-ConditionalFormatting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rm77\Desktop\Test\1910\Reports\Logistic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rm77\Desktop\ТЕСТ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16D79EE-9995-4C01-B37B-AF98C2CF54F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCEED18-C331-40FB-9B0F-D500F22F95A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Rows">Лист1!$B$7:$AN$8</definedName>
+    <definedName name="DaysNumbers">Лист1!$J$6</definedName>
+    <definedName name="Rows">Лист1!$B$7:$K$8</definedName>
     <definedName name="Rows_Days">Лист1!$J$7</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Аналитика эксплуатации ТС за {{StartDate.ToString("MM-yyyy")}}г.</t>
   </si>
@@ -43,12 +44,6 @@
     <t>{{CreationDate}}</t>
   </si>
   <si>
-    <t>Выбранные фильтры: {{Filters}}</t>
-  </si>
-  <si>
-    <t>Сформировано: {{CreationDate.ToString()}}</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -104,6 +99,10 @@
   </si>
   <si>
     <t>Итого</t>
+  </si>
+  <si>
+    <t>Сформировано: {{CreationDate.ToString()}}
+Выбранные фильтры: {{Filters}}</t>
   </si>
 </sst>
 </file>
@@ -231,7 +230,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -253,12 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,9 +264,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -281,18 +271,11 @@
     <cellStyle name="Hidden" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -339,21 +322,29 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -361,33 +352,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -412,6 +376,69 @@
         <color rgb="FF000000"/>
         <name val="Calibri"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -757,9 +784,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AO7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -770,311 +799,148 @@
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="10" max="40" width="6.42578125" customWidth="1"/>
-    <col min="41" max="41" width="8.42578125" customWidth="1"/>
-    <col min="42" max="42" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:41" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="AJ2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="AN3" s="1" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:11" ht="113.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
-    <row r="4" spans="2:41" ht="113.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="2:41" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="7">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7">
-        <v>3</v>
-      </c>
-      <c r="M6" s="7">
-        <v>4</v>
-      </c>
-      <c r="N6" s="7">
-        <v>5</v>
-      </c>
-      <c r="O6" s="7">
-        <v>6</v>
-      </c>
-      <c r="P6" s="7">
-        <v>7</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>8</v>
-      </c>
-      <c r="R6" s="7">
-        <v>9</v>
-      </c>
-      <c r="S6" s="7">
-        <v>10</v>
-      </c>
-      <c r="T6" s="7">
-        <v>11</v>
-      </c>
-      <c r="U6" s="7">
-        <v>12</v>
-      </c>
-      <c r="V6" s="7">
-        <v>13</v>
-      </c>
-      <c r="W6" s="7">
+      <c r="E7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="7">
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="H7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="I7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AA6" s="7">
+      <c r="J7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AB6" s="7">
-        <v>19</v>
-      </c>
-      <c r="AC6" s="7">
+      <c r="K7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AD6" s="7">
-        <v>21</v>
-      </c>
-      <c r="AE6" s="7">
-        <v>22</v>
-      </c>
-      <c r="AF6" s="7">
-        <v>23</v>
-      </c>
-      <c r="AG6" s="7">
-        <v>24</v>
-      </c>
-      <c r="AH6" s="7">
-        <v>25</v>
-      </c>
-      <c r="AI6" s="7">
-        <v>26</v>
-      </c>
-      <c r="AJ6" s="7">
-        <v>27</v>
-      </c>
-      <c r="AK6" s="7">
-        <v>28</v>
-      </c>
-      <c r="AL6" s="7">
-        <v>29</v>
-      </c>
-      <c r="AM6" s="7">
-        <v>30</v>
-      </c>
-      <c r="AN6" s="7">
-        <v>31</v>
-      </c>
-      <c r="AO6" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="9"/>
-      <c r="AN7" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:W2"/>
-    <mergeCell ref="AJ2:AM2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:AN4"/>
   </mergeCells>
-  <conditionalFormatting sqref="J6:AN6">
-    <cfRule type="expression" dxfId="14" priority="11">
-      <formula>WEEKDAY($AJ$2+J6-2)&gt;5</formula>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="expression" dxfId="13" priority="4">
+      <formula>$G7="Всего"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>WEEKDAY($A$1+J6-2)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>$G7="Всего"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>$AN$3 &lt; $AJ$2+J$6-1</formula>
+    <cfRule type="expression" dxfId="10" priority="24">
+      <formula>$F$1 &lt; $A$1+J$6-1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
-      <formula>AND($G7="Рейсы",IF($E7="Л",J7&lt;2,J7&lt;1))</formula>
+    <cfRule type="expression" dxfId="8" priority="25">
+      <formula>AND($G7="Рейсы",IF($E7="Л",J7&lt;2,J7&lt;1),J$6&lt;&gt;"Итого")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="15">
-      <formula>AND($G7="Город/Пригород",AND($D7="К",J7="П"))</formula>
+    <cfRule type="expression" dxfId="7" priority="26">
+      <formula>AND($G7="Город/Пригород",AND($D7="К",J7="П"),J$6&lt;&gt;"Итого")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>$G7="Всего"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="1">
-      <formula>$G7&lt;&gt;"Всего"</formula>
+    <cfRule type="expression" dxfId="9" priority="23">
+      <formula>J$6="Итого"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>